<commit_message>
märgendajad ja neile antud failide tabel
</commit_message>
<xml_diff>
--- a/syntax/verb_rections/location_phrases/annotation_task_01/margendajad.xlsx
+++ b/syntax/verb_rections/location_phrases/annotation_task_01/margendajad.xlsx
@@ -28,37 +28,37 @@
     <t xml:space="preserve">andmestik</t>
   </si>
   <si>
-    <t xml:space="preserve">Annaliis Tenisson</t>
+    <t xml:space="preserve">Annaliis</t>
   </si>
   <si>
     <t xml:space="preserve">abl_set1</t>
   </si>
   <si>
-    <t xml:space="preserve">Kertu Zahharov</t>
+    <t xml:space="preserve">Kertu</t>
   </si>
   <si>
     <t xml:space="preserve">ad_set1</t>
   </si>
   <si>
-    <t xml:space="preserve">Andrea Nagy</t>
+    <t xml:space="preserve">Andrea</t>
   </si>
   <si>
     <t xml:space="preserve">all_set1</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiia Margus</t>
+    <t xml:space="preserve">Tiia</t>
   </si>
   <si>
     <t xml:space="preserve">el_set1</t>
   </si>
   <si>
-    <t xml:space="preserve">Agnes Lea</t>
+    <t xml:space="preserve">Agnes</t>
   </si>
   <si>
     <t xml:space="preserve">ill_set1</t>
   </si>
   <si>
-    <t xml:space="preserve">Käbi Laan</t>
+    <t xml:space="preserve">Käbi</t>
   </si>
   <si>
     <t xml:space="preserve">in_set1</t>
@@ -76,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,10 +172,10 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.61"/>
   </cols>

</xml_diff>